<commit_message>
finished the IKSA reasaerch and also the lomonosov 2025 presentation
</commit_message>
<xml_diff>
--- a/IKSA/china_cobb_douglas_data.xlsx
+++ b/IKSA/china_cobb_douglas_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="146">
   <si>
     <t>Country Name</t>
   </si>
@@ -462,16 +462,16 @@
     <t>Capital stock (current US$)</t>
   </si>
   <si>
-    <t>Captial stock (current LCU)</t>
-  </si>
-  <si>
     <t>CAPSTO.CD.5%</t>
   </si>
   <si>
     <t>CAPSTO.CN.5%</t>
   </si>
   <si>
-    <t>Calculated starting from 1978 . The initial 1978 Capital Stock was calculated by dividing the GFCF in 1978 and dividing it by the sum of the average growth rate of GFCF 1960-1978 and a depriciation rate of 5%. Afterwards each following year's capital stock was calculated by taking the depricated value of the previous year (K[t-1]*0.95) and adding the current years GFCF.</t>
+    <t>Capital stock (current LCU)</t>
+  </si>
+  <si>
+    <t>Calculated starting from 1978 . The initial 1978 Capital Stock was calculated by dividing the GFCF in 1978 and dividing it by the sum of the average growth rate of GFCF 1960-1978 and a depriciation rate of 5%). Afterwards each following year's capital stock was calculated by taking the depricated value of the previous year (K*0.95) and adding the current years GFCF.</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -525,13 +525,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -813,31 +814,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS19"/>
+  <dimension ref="A1:BR19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="BJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD8" sqref="AD8"/>
+      <selection pane="bottomRight" activeCell="BO8" sqref="BO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="40" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="55" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="67" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="22" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="37" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="51" width="20" bestFit="1" customWidth="1"/>
+    <col min="52" max="68" width="21" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,9 +1045,9 @@
       <c r="BQ1" t="s">
         <v>139</v>
       </c>
-      <c r="BS1" s="2"/>
+      <c r="BR1" s="2"/>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>143</v>
@@ -1079,147 +1079,149 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="5">
-        <v>433067532047.06274</v>
+        <v>875189248321.74243</v>
       </c>
       <c r="X2" s="5">
-        <v>486180230227.65381</v>
+        <v>947683555585.65527</v>
       </c>
       <c r="Y2" s="5">
-        <v>549313910220.54236</v>
+        <v>1031323506756.3724</v>
       </c>
       <c r="Z2" s="5">
-        <v>600780171318.49146</v>
+        <v>1114296851458.5537</v>
       </c>
       <c r="AA2" s="5">
-        <v>650920971323.2406</v>
+        <v>1210322296605.626</v>
       </c>
       <c r="AB2" s="5">
-        <v>704244840907.60742</v>
+        <v>1319459379065.3447</v>
       </c>
       <c r="AC2" s="5">
-        <v>761021093892.39941</v>
+        <v>1466899718582.0774</v>
       </c>
       <c r="AD2" s="5">
-        <v>817256918467.02722</v>
+        <v>1670447011002.9734</v>
       </c>
       <c r="AE2" s="5">
-        <v>869431953845.80737</v>
+        <v>1908165857012.8247</v>
       </c>
       <c r="AF2" s="5">
-        <v>925913765298.89185</v>
+        <v>2184794148342.1833</v>
       </c>
       <c r="AG2" s="5">
-        <v>1006265356634.173</v>
+        <v>2546948280325.0742</v>
       </c>
       <c r="AH2" s="5">
-        <v>1072789790111.8584</v>
+        <v>2859506495508.8203</v>
       </c>
       <c r="AI2" s="5">
-        <v>1113801705701.1809</v>
+        <v>3169267771583.3794</v>
       </c>
       <c r="AJ2" s="5">
-        <v>1164364813394.2937</v>
+        <v>3576432630504.2104</v>
       </c>
       <c r="AK2" s="5">
-        <v>1255800422831.5676</v>
+        <v>4222892120779</v>
       </c>
       <c r="AL2" s="5">
-        <v>1422652847351.218</v>
+        <v>5334947286640.0498</v>
       </c>
       <c r="AM2" s="5">
-        <v>1545876130273.4585</v>
+        <v>6743303692908.0469</v>
       </c>
       <c r="AN2" s="5">
-        <v>1706121834994.825</v>
+        <v>8389930020562.6445</v>
       </c>
       <c r="AO2" s="5">
-        <v>1894123342339.4016</v>
+        <v>10242760727234.512</v>
       </c>
       <c r="AP2" s="5">
-        <v>2097543562475.6121</v>
+        <v>12202035884072.785</v>
       </c>
       <c r="AQ2" s="5">
-        <v>2331048258012.7437</v>
+        <v>14393383409869.145</v>
       </c>
       <c r="AR2" s="5">
-        <v>2570455413073.7407</v>
+        <v>16620418734875.688</v>
       </c>
       <c r="AS2" s="5">
-        <v>2836553213056.9707</v>
+        <v>19056265770631.902</v>
       </c>
       <c r="AT2" s="5">
-        <v>3142802384731.7046</v>
+        <v>21812214892500.305</v>
       </c>
       <c r="AU2" s="5">
-        <v>3501215751117.915</v>
+        <v>24988818179575.289</v>
       </c>
       <c r="AV2" s="5">
-        <v>3961339869597.8384</v>
+        <v>28996826239696.523</v>
       </c>
       <c r="AW2" s="5">
-        <v>4536214878493.0186</v>
+        <v>33944472065911.695</v>
       </c>
       <c r="AX2" s="5">
-        <v>5210662961472.4277</v>
+        <v>39632448989316.109</v>
       </c>
       <c r="AY2" s="5">
-        <v>6015901196596.3672</v>
+        <v>46148688585950.305</v>
       </c>
       <c r="AZ2" s="5">
-        <v>7060412975436.4355</v>
+        <v>54075718981352.789</v>
       </c>
       <c r="BA2" s="5">
-        <v>8501994400447.2373</v>
+        <v>63842003705185.148</v>
       </c>
       <c r="BB2" s="5">
-        <v>10312025710507.072</v>
+        <v>75919013400925.891</v>
       </c>
       <c r="BC2" s="5">
-        <v>12470485439248.656</v>
+        <v>90227175119679.594</v>
       </c>
       <c r="BD2" s="5">
-        <v>15159171924419.941</v>
+        <v>107117536994295.61</v>
       </c>
       <c r="BE2" s="5">
-        <v>18176691024638.594</v>
+        <v>125593732598180.83</v>
       </c>
       <c r="BF2" s="5">
-        <v>21528512069703.355</v>
+        <v>145712036964471.78</v>
       </c>
       <c r="BG2" s="5">
-        <v>25046286357679.543</v>
+        <v>166650598931948.19</v>
       </c>
       <c r="BH2" s="5">
-        <v>28450266730320.109</v>
+        <v>187315092951150.78</v>
       </c>
       <c r="BI2" s="5">
-        <v>31695460907923.344</v>
+        <v>208963818191193.22</v>
       </c>
       <c r="BJ2" s="5">
-        <v>35264005450899.594</v>
+        <v>233345638298833.56</v>
       </c>
       <c r="BK2" s="5">
-        <v>39453804878322.438</v>
+        <v>261063146419391.88</v>
       </c>
       <c r="BL2" s="5">
-        <v>43596166193345.195</v>
+        <v>290255119562022.25</v>
       </c>
       <c r="BM2" s="5">
-        <v>47656604405550.07</v>
+        <v>318804850853921.13</v>
       </c>
       <c r="BN2" s="5">
-        <v>52749680415022.25</v>
+        <v>351076540689025.06</v>
       </c>
       <c r="BO2" s="5">
-        <v>57651837661464.211</v>
-      </c>
-      <c r="BP2" s="4"/>
+        <v>384006178041343.81</v>
+      </c>
+      <c r="BP2" s="5">
+        <v>416917100613076.63</v>
+      </c>
       <c r="BQ2" t="s">
         <v>145</v>
       </c>
-      <c r="BS2" s="2"/>
+      <c r="BR2" s="2"/>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1227,10 +1229,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1251,147 +1253,149 @@
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="5">
-        <v>875189248321.74243</v>
+        <v>350477636715.52887</v>
       </c>
       <c r="X3" s="5">
-        <v>947683555585.65527</v>
+        <v>383498872131.92627</v>
       </c>
       <c r="Y3" s="5">
-        <v>1031323506756.3724</v>
+        <v>418917315587.82996</v>
       </c>
       <c r="Z3" s="5">
-        <v>1114296851458.5537</v>
+        <v>451360148237.00983</v>
       </c>
       <c r="AA3" s="5">
-        <v>1210322296605.626</v>
+        <v>486708281176.30432</v>
       </c>
       <c r="AB3" s="5">
-        <v>1319459379065.3447</v>
+        <v>527374092132.81476</v>
       </c>
       <c r="AC3" s="5">
-        <v>1466899718582.0774</v>
+        <v>577224426265.45972</v>
       </c>
       <c r="AD3" s="5">
-        <v>1670447011002.9734</v>
+        <v>642544252010.00989</v>
       </c>
       <c r="AE3" s="5">
-        <v>1908165857012.8247</v>
+        <v>703530429716.75574</v>
       </c>
       <c r="AF3" s="5">
-        <v>2184794148342.1833</v>
+        <v>751770182710.73865</v>
       </c>
       <c r="AG3" s="5">
-        <v>2546948280325.0742</v>
+        <v>811176290735.69543</v>
       </c>
       <c r="AH3" s="5">
-        <v>2859506495508.8203</v>
+        <v>859667198709.0321</v>
       </c>
       <c r="AI3" s="5">
-        <v>3169267771583.3794</v>
+        <v>903249154423.67603</v>
       </c>
       <c r="AJ3" s="5">
-        <v>3576432630504.2104</v>
+        <v>956628203235.59326</v>
       </c>
       <c r="AK3" s="5">
-        <v>4222892120779</v>
+        <v>1038354269023.5781</v>
       </c>
       <c r="AL3" s="5">
-        <v>5334947286640.0498</v>
+        <v>1151397319027.2007</v>
       </c>
       <c r="AM3" s="5">
-        <v>6743303692908.0469</v>
+        <v>1288183378365.6421</v>
       </c>
       <c r="AN3" s="5">
-        <v>8389930020562.6445</v>
+        <v>1461313720682.3994</v>
       </c>
       <c r="AO3" s="5">
-        <v>10242760727234.512</v>
+        <v>1661555633742.5972</v>
       </c>
       <c r="AP3" s="5">
-        <v>12202035884072.785</v>
+        <v>1876604239308.6479</v>
       </c>
       <c r="AQ3" s="5">
-        <v>14393383409869.145</v>
+        <v>2121155901004.1279</v>
       </c>
       <c r="AR3" s="5">
-        <v>16620418734875.688</v>
+        <v>2371055523946.8545</v>
       </c>
       <c r="AS3" s="5">
-        <v>19056265770631.902</v>
+        <v>2647123318386.4287</v>
       </c>
       <c r="AT3" s="5">
-        <v>21812214892500.305</v>
+        <v>2962843984794.6895</v>
       </c>
       <c r="AU3" s="5">
-        <v>24988818179575.289</v>
+        <v>3330255271177.751</v>
       </c>
       <c r="AV3" s="5">
-        <v>28996826239696.523</v>
+        <v>3798927413654.6826</v>
       </c>
       <c r="AW3" s="5">
-        <v>33944472065911.695</v>
+        <v>4381923045347.0205</v>
       </c>
       <c r="AX3" s="5">
-        <v>39632448989316.109</v>
+        <v>5064085719983.7295</v>
       </c>
       <c r="AY3" s="5">
-        <v>46148688585950.305</v>
+        <v>5876652817182.1045</v>
       </c>
       <c r="AZ3" s="5">
-        <v>54075718981652.789</v>
+        <v>6928127014953.4512</v>
       </c>
       <c r="BA3" s="5">
-        <v>63842003705570.148</v>
+        <v>8376322737974.0117</v>
       </c>
       <c r="BB3" s="5">
-        <v>75919013401291.641</v>
+        <v>10192637631157.508</v>
       </c>
       <c r="BC3" s="5">
-        <v>90227175120227.063</v>
+        <v>12357066763837.029</v>
       </c>
       <c r="BD3" s="5">
-        <v>107117536995215.7</v>
+        <v>15051424182716.992</v>
       </c>
       <c r="BE3" s="5">
-        <v>125593732599454.91</v>
+        <v>18074330669957.426</v>
       </c>
       <c r="BF3" s="5">
-        <v>145712036965482.16</v>
+        <v>21431269732788.523</v>
       </c>
       <c r="BG3" s="5">
-        <v>166650598933208.06</v>
+        <v>24953906137561.621</v>
       </c>
       <c r="BH3" s="5">
-        <v>187315092952547.66</v>
+        <v>28362505521175.969</v>
       </c>
       <c r="BI3" s="5">
-        <v>208963818192920.25</v>
+        <v>31612087759176.211</v>
       </c>
       <c r="BJ3" s="5">
-        <v>233345638300274.22</v>
+        <v>35184800959619.406</v>
       </c>
       <c r="BK3" s="5">
-        <v>261063146421260.5</v>
+        <v>39378560611530.68</v>
       </c>
       <c r="BL3" s="5">
-        <v>290255119564197.5</v>
+        <v>43524684139835.125</v>
       </c>
       <c r="BM3" s="5">
-        <v>318804850855987.63</v>
+        <v>47588696454715.5</v>
       </c>
       <c r="BN3" s="5">
-        <v>351076540691188.25</v>
+        <v>52685167861698.406</v>
       </c>
       <c r="BO3" s="5">
-        <v>384318468137028.81</v>
-      </c>
-      <c r="BP3" s="4"/>
+        <v>57544197348572.656</v>
+      </c>
+      <c r="BP3" s="5">
+        <v>62023176948419.422</v>
+      </c>
       <c r="BQ3" t="s">
         <v>145</v>
       </c>
-      <c r="BS3" s="2"/>
+      <c r="BR3" s="2"/>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1399,204 +1403,206 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4">
-        <v>19495171136.347294</v>
+        <v>158907448897.85104</v>
       </c>
       <c r="F4" s="4">
-        <v>9506393846.9637566</v>
+        <v>115573387577.22798</v>
       </c>
       <c r="G4" s="4">
-        <v>7307599407.5901089</v>
+        <v>109124392561.74864</v>
       </c>
       <c r="H4" s="4">
-        <v>9003677226.7872925</v>
+        <v>120364204991.67909</v>
       </c>
       <c r="I4" s="4">
-        <v>12100169923.824308</v>
+        <v>142246417451.72818</v>
       </c>
       <c r="J4" s="4">
-        <v>14539666818.181263</v>
+        <v>166357185215.30154</v>
       </c>
       <c r="K4" s="4">
-        <v>16743508489.082621</v>
+        <v>184074225438.09799</v>
       </c>
       <c r="L4" s="4">
-        <v>13248090245.831419</v>
+        <v>173453142622.86108</v>
       </c>
       <c r="M4" s="4">
-        <v>12303878586.844065</v>
+        <v>166341563798.77902</v>
       </c>
       <c r="N4" s="4">
-        <v>16724341920.920753</v>
+        <v>194519824699.7403</v>
       </c>
       <c r="O4" s="4">
-        <v>22354514935.967819</v>
+        <v>232062150860.3757</v>
       </c>
       <c r="P4" s="4">
-        <v>24796716479.62941</v>
+        <v>248445738707.72202</v>
       </c>
       <c r="Q4" s="4">
-        <v>27998375041.090107</v>
+        <v>257911521353.0321</v>
       </c>
       <c r="R4" s="4">
-        <v>33644743794.158684</v>
+        <v>277925455412.20172</v>
       </c>
       <c r="S4" s="4">
-        <v>38293247655.533333</v>
+        <v>284345533440.41522</v>
       </c>
       <c r="T4" s="4">
-        <v>47472832936.252533</v>
+        <v>309140463949.25415</v>
       </c>
       <c r="U4" s="4">
-        <v>44699652856.292961</v>
+        <v>304286958660.13971</v>
       </c>
       <c r="V4" s="4">
-        <v>49200930266.230957</v>
+        <v>327321481434.92358</v>
       </c>
       <c r="W4" s="4">
-        <v>64108603171.774773</v>
+        <v>364393840371.8764</v>
       </c>
       <c r="X4" s="4">
-        <v>74766074782.944244</v>
+        <v>392056159908.45831</v>
       </c>
       <c r="Y4" s="4">
-        <v>87442691504.271225</v>
+        <v>422770408019.50476</v>
       </c>
       <c r="Z4" s="4">
-        <v>78931956608.976242</v>
+        <v>444385648943.33807</v>
       </c>
       <c r="AA4" s="4">
-        <v>80179808570.673706</v>
+        <v>484456409125.22278</v>
       </c>
       <c r="AB4" s="4">
-        <v>85869918150.528931</v>
+        <v>536633345444.08447</v>
       </c>
       <c r="AC4" s="4">
-        <v>91988495030.172424</v>
+        <v>618156214897.21008</v>
       </c>
       <c r="AD4" s="4">
-        <v>94286879269.247787</v>
+        <v>701178782692.45532</v>
       </c>
       <c r="AE4" s="4">
-        <v>93037881302.131607</v>
+        <v>763934015643.45313</v>
       </c>
       <c r="AF4" s="4">
-        <v>99953409145.374924</v>
+        <v>852989071904.21399</v>
       </c>
       <c r="AG4" s="4">
-        <v>126647279600.22568</v>
+        <v>948716580689.1886</v>
       </c>
       <c r="AH4" s="4">
-        <v>116837701309.39418</v>
+        <v>988622772158.87769</v>
       </c>
       <c r="AI4" s="4">
-        <v>94651405094.915543</v>
+        <v>1027379269906.5031</v>
       </c>
       <c r="AJ4" s="4">
-        <v>106253192978.17184</v>
+        <v>1122543213961.2842</v>
       </c>
       <c r="AK4" s="4">
-        <v>149653850106.98874</v>
+        <v>1282219705619.7678</v>
       </c>
       <c r="AL4" s="4">
-        <v>229642445661.22876</v>
+        <v>1460239618602.0059</v>
       </c>
       <c r="AM4" s="4">
-        <v>194355925289.80154</v>
+        <v>1650608234052.8538</v>
       </c>
       <c r="AN4" s="4">
-        <v>237539511235.03952</v>
+        <v>1831415106374.645</v>
       </c>
       <c r="AO4" s="4">
-        <v>273307599094.31781</v>
+        <v>2013138309684.4414</v>
       </c>
       <c r="AP4" s="4">
-        <v>298126387253.18066</v>
+        <v>2199087464269.0137</v>
       </c>
       <c r="AQ4" s="4">
-        <v>338381873660.91241</v>
+        <v>2371626806476.0879</v>
       </c>
       <c r="AR4" s="4">
-        <v>355959567961.63416</v>
+        <v>2553332587278.4253</v>
       </c>
       <c r="AS4" s="4">
-        <v>394620570636.91699</v>
+        <v>2770112908903.5991</v>
       </c>
       <c r="AT4" s="4">
-        <v>448076832327.5827</v>
+        <v>3001022138034.2393</v>
       </c>
       <c r="AU4" s="4">
-        <v>515553485622.79596</v>
+        <v>3275124420038.4321</v>
       </c>
       <c r="AV4" s="4">
-        <v>635184906035.81934</v>
+        <v>3603882407613.8516</v>
       </c>
       <c r="AW4" s="4">
-        <v>772942002375.07214</v>
+        <v>3968365429214.8003</v>
       </c>
       <c r="AX4" s="4">
-        <v>901258826904.06042</v>
+        <v>4420544471398.7217</v>
       </c>
       <c r="AY4" s="4">
-        <v>1065771383197.5618</v>
+        <v>4982879973774.7852</v>
       </c>
       <c r="AZ4" s="4">
-        <v>1345306838669.8867</v>
+        <v>5691986693310.7256</v>
       </c>
       <c r="BA4" s="4">
-        <v>1794602073782.6243</v>
+        <v>6241302053216.7539</v>
       </c>
       <c r="BB4" s="4">
-        <v>2235131030082.1968</v>
+        <v>6827904909100.2236</v>
       </c>
       <c r="BC4" s="4">
-        <v>2674061014266.937</v>
+        <v>7554112071638.1963</v>
       </c>
       <c r="BD4" s="4">
-        <v>3312210757133.7197</v>
+        <v>8275592638196.9951</v>
       </c>
       <c r="BE4" s="4">
-        <v>3775477696439.6523</v>
+        <v>8926363432826.2969</v>
       </c>
       <c r="BF4" s="4">
-        <v>4260655596296.6924</v>
+        <v>9619598215288.4805</v>
       </c>
       <c r="BG4" s="4">
-        <v>4594199891461.3555</v>
+        <v>10333926843443.777</v>
       </c>
       <c r="BH4" s="4">
-        <v>4656294690524.5439</v>
+        <v>11061572618578.693</v>
       </c>
       <c r="BI4" s="4">
-        <v>4667707514119.2432</v>
+        <v>11819153423353.85</v>
       </c>
       <c r="BJ4" s="4">
-        <v>5153317588372.4141</v>
+        <v>12640253743744.424</v>
       </c>
       <c r="BK4" s="4">
-        <v>5952999699967.8203</v>
+        <v>13493442283300.77</v>
       </c>
       <c r="BL4" s="4">
-        <v>6115051558938.8838</v>
+        <v>14296369668065.166</v>
       </c>
       <c r="BM4" s="4">
-        <v>6240246521872.1338</v>
+        <v>14616413683019.543</v>
       </c>
       <c r="BN4" s="4">
-        <v>7475906229749.6895</v>
+        <v>15851276922873.055</v>
       </c>
       <c r="BO4" s="4">
-        <v>7539641267193.0801</v>
-      </c>
-      <c r="BP4" s="4"/>
-      <c r="BS4" s="2"/>
+        <v>16318995784492.732</v>
+      </c>
+      <c r="BP4" s="4">
+        <v>17175670911003.475</v>
+      </c>
+      <c r="BR4" s="2"/>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1604,204 +1610,206 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4">
-        <v>47993387760</v>
+        <v>1101934784445</v>
       </c>
       <c r="F5" s="4">
-        <v>23402925930</v>
+        <v>801437168684</v>
       </c>
       <c r="G5" s="4">
-        <v>17989913990</v>
+        <v>756716974750</v>
       </c>
       <c r="H5" s="4">
-        <v>22165333630</v>
+        <v>834658823122</v>
       </c>
       <c r="I5" s="4">
-        <v>29788307220</v>
+        <v>986399797114</v>
       </c>
       <c r="J5" s="4">
-        <v>35793882630</v>
+        <v>1153594562763</v>
       </c>
       <c r="K5" s="4">
-        <v>41219319890</v>
+        <v>1276452383679</v>
       </c>
       <c r="L5" s="4">
-        <v>32614267800</v>
+        <v>1202801081089</v>
       </c>
       <c r="M5" s="4">
-        <v>30289799040</v>
+        <v>1153486236927</v>
       </c>
       <c r="N5" s="4">
-        <v>41172135460</v>
+        <v>1348886805417</v>
       </c>
       <c r="O5" s="4">
-        <v>55032546060</v>
+        <v>1609221958818</v>
       </c>
       <c r="P5" s="4">
-        <v>61044779800</v>
+        <v>1722833029087</v>
       </c>
       <c r="Q5" s="4">
-        <v>62858199860</v>
+        <v>1788472967499</v>
       </c>
       <c r="R5" s="4">
-        <v>66933391619.999992</v>
+        <v>1927258469792</v>
       </c>
       <c r="S5" s="4">
-        <v>75097156030</v>
+        <v>1971778140501</v>
       </c>
       <c r="T5" s="4">
-        <v>88291066570</v>
+        <v>2143717194303</v>
       </c>
       <c r="U5" s="4">
-        <v>86780576550</v>
+        <v>2110060834317</v>
       </c>
       <c r="V5" s="4">
-        <v>91406619870</v>
+        <v>2269792439504</v>
       </c>
       <c r="W5" s="4">
-        <v>107933244300</v>
+        <v>2526868631573</v>
       </c>
       <c r="X5" s="4">
-        <v>116253769680</v>
+        <v>2718691433633</v>
       </c>
       <c r="Y5" s="4">
-        <v>131024128950</v>
+        <v>2931677663079</v>
       </c>
       <c r="Z5" s="4">
-        <v>134539520040</v>
+        <v>3081567337939</v>
       </c>
       <c r="AA5" s="4">
-        <v>151740287720</v>
+        <v>3359435775132</v>
       </c>
       <c r="AB5" s="4">
-        <v>169653197290</v>
+        <v>3721253811192</v>
       </c>
       <c r="AC5" s="4">
-        <v>213413308470</v>
+        <v>4286569573299</v>
       </c>
       <c r="AD5" s="4">
-        <v>276892278350</v>
+        <v>4862284909377</v>
       </c>
       <c r="AE5" s="4">
-        <v>321241196560</v>
+        <v>5297457549642</v>
       </c>
       <c r="AF5" s="4">
-        <v>372036584180</v>
+        <v>5915004838363</v>
       </c>
       <c r="AG5" s="4">
-        <v>471393839400</v>
+        <v>6578821874569</v>
       </c>
       <c r="AH5" s="4">
-        <v>439905629200</v>
+        <v>6855549119265</v>
       </c>
       <c r="AI5" s="4">
-        <v>452736600850</v>
+        <v>7124303877381</v>
       </c>
       <c r="AJ5" s="4">
-        <v>565628247500</v>
+        <v>7784212905600</v>
       </c>
       <c r="AK5" s="4">
-        <v>825281121800</v>
+        <v>8891480573900</v>
       </c>
       <c r="AL5" s="4">
-        <v>1323199771900</v>
+        <v>10125949667700</v>
       </c>
       <c r="AM5" s="4">
-        <v>1675103770600</v>
+        <v>11446050145600</v>
       </c>
       <c r="AN5" s="4">
-        <v>1983791512300</v>
+        <v>12699845252500</v>
       </c>
       <c r="AO5" s="4">
-        <v>2272327207700</v>
+        <v>13959994605200</v>
       </c>
       <c r="AP5" s="4">
-        <v>2471413193200</v>
+        <v>15249448579800</v>
       </c>
       <c r="AQ5" s="4">
-        <v>2801449320000</v>
+        <v>16445912963200</v>
       </c>
       <c r="AR5" s="4">
-        <v>2946704495500</v>
+        <v>17705941500500</v>
       </c>
       <c r="AS5" s="4">
-        <v>3266867972500</v>
+        <v>19209192472300</v>
       </c>
       <c r="AT5" s="4">
-        <v>3708762410400</v>
+        <v>20810419560100</v>
       </c>
       <c r="AU5" s="4">
-        <v>4267214031700</v>
+        <v>22711166448500</v>
       </c>
       <c r="AV5" s="4">
-        <v>5257448969100</v>
+        <v>24990920259200</v>
       </c>
       <c r="AW5" s="4">
-        <v>6397487138200</v>
+        <v>27518407313000</v>
       </c>
       <c r="AX5" s="4">
-        <v>7385200526700</v>
+        <v>30654017498900</v>
       </c>
       <c r="AY5" s="4">
-        <v>8497862046100</v>
+        <v>34553501474600.004</v>
       </c>
       <c r="AZ5" s="4">
-        <v>10234464825000</v>
+        <v>39470762217000</v>
       </c>
       <c r="BA5" s="4">
-        <v>12470070673000</v>
+        <v>43279958745600</v>
       </c>
       <c r="BB5" s="4">
-        <v>15269109881000</v>
+        <v>47347723322000</v>
       </c>
       <c r="BC5" s="4">
-        <v>18104112389000</v>
+        <v>52383566126500</v>
       </c>
       <c r="BD5" s="4">
-        <v>21401720631000</v>
+        <v>57386632616500</v>
       </c>
       <c r="BE5" s="4">
-        <v>23832072454000</v>
+        <v>61899366162200</v>
       </c>
       <c r="BF5" s="4">
-        <v>26397990996000</v>
+        <v>66706563847900</v>
       </c>
       <c r="BG5" s="4">
-        <v>28224163816000</v>
+        <v>71660035622500</v>
       </c>
       <c r="BH5" s="4">
-        <v>28997023966000</v>
+        <v>76705854405300</v>
       </c>
       <c r="BI5" s="4">
-        <v>31014479888000</v>
+        <v>81959255970800</v>
       </c>
       <c r="BJ5" s="4">
-        <v>34830011016999.996</v>
+        <v>87653130051800</v>
       </c>
       <c r="BK5" s="4">
-        <v>39384790036000</v>
+        <v>93569518087400</v>
       </c>
       <c r="BL5" s="4">
-        <v>42245130464000</v>
+        <v>99137372966400</v>
       </c>
       <c r="BM5" s="4">
-        <v>43062487270000</v>
+        <v>101356700223100</v>
       </c>
       <c r="BN5" s="4">
-        <v>48211932378000</v>
+        <v>109919790043400</v>
       </c>
       <c r="BO5" s="4">
-        <v>50795754480400</v>
-      </c>
-      <c r="BP5" s="4"/>
-      <c r="BS5" s="2"/>
+        <v>113163160234882</v>
+      </c>
+      <c r="BP5" s="4">
+        <v>119103725812005</v>
+      </c>
+      <c r="BR5" s="2"/>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1809,204 +1817,206 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4">
-        <v>59716249310.974159</v>
+        <v>147010000000</v>
       </c>
       <c r="F6" s="4">
-        <v>50056685957.358994</v>
+        <v>123230000000</v>
       </c>
       <c r="G6" s="4">
-        <v>47209186415.355537</v>
+        <v>116220000000</v>
       </c>
       <c r="H6" s="4">
-        <v>50706614526.147232</v>
+        <v>124830000000</v>
       </c>
       <c r="I6" s="4">
-        <v>59708125203.864311</v>
+        <v>146990000000</v>
       </c>
       <c r="J6" s="4">
-        <v>70436008642.42514</v>
+        <v>173400000000</v>
       </c>
       <c r="K6" s="4">
-        <v>76720005491.896408</v>
+        <v>188870000000</v>
       </c>
       <c r="L6" s="4">
-        <v>72881364882.490875</v>
+        <v>179420000000</v>
       </c>
       <c r="M6" s="4">
-        <v>70846276051.472717</v>
+        <v>174410000000</v>
       </c>
       <c r="N6" s="4">
-        <v>79705614854.767365</v>
+        <v>196220000000</v>
       </c>
       <c r="O6" s="4">
-        <v>92602634891.658936</v>
+        <v>227970000000</v>
       </c>
       <c r="P6" s="4">
-        <v>99800593790.988647</v>
+        <v>245690000000</v>
       </c>
       <c r="Q6" s="4">
-        <v>113689308020.34328</v>
+        <v>255240000000</v>
       </c>
       <c r="R6" s="4">
-        <v>138543170458.06406</v>
+        <v>275620000000</v>
       </c>
       <c r="S6" s="4">
-        <v>144188970821.07199</v>
+        <v>282770000000</v>
       </c>
       <c r="T6" s="4">
-        <v>163429530659.63803</v>
+        <v>303950000000</v>
       </c>
       <c r="U6" s="4">
-        <v>153939265947.77521</v>
+        <v>298860000000</v>
       </c>
       <c r="V6" s="4">
-        <v>174935933078.66251</v>
+        <v>325000000000</v>
       </c>
       <c r="W6" s="4">
-        <v>218502169137.56238</v>
+        <v>367870251960</v>
       </c>
       <c r="X6" s="4">
-        <v>263711728825.00482</v>
+        <v>410045367150</v>
       </c>
       <c r="Y6" s="4">
-        <v>306165314855.84625</v>
+        <v>458758107780</v>
       </c>
       <c r="Z6" s="4">
-        <v>289576581830.44885</v>
+        <v>493583283730</v>
       </c>
       <c r="AA6" s="4">
-        <v>283928672988.1109</v>
+        <v>537335013629.99994</v>
       </c>
       <c r="AB6" s="4">
-        <v>304748904221.28864</v>
+        <v>602092410070</v>
       </c>
       <c r="AC6" s="4">
-        <v>313728547706.89655</v>
+        <v>727850230680</v>
       </c>
       <c r="AD6" s="4">
-        <v>309835803013.58667</v>
+        <v>909894802710</v>
       </c>
       <c r="AE6" s="4">
-        <v>300514204520.96851</v>
+        <v>1037615445370</v>
       </c>
       <c r="AF6" s="4">
-        <v>327089403146.07343</v>
+        <v>1217459467450</v>
       </c>
       <c r="AG6" s="4">
-        <v>407844670393.05768</v>
+        <v>1518038647670</v>
       </c>
       <c r="AH6" s="4">
-        <v>456289122063.159</v>
+        <v>1717974173480</v>
       </c>
       <c r="AI6" s="4">
-        <v>394565747349.05505</v>
+        <v>1887286882720</v>
       </c>
       <c r="AJ6" s="4">
-        <v>413375445354.47266</v>
+        <v>2200562845800</v>
       </c>
       <c r="AK6" s="4">
-        <v>493136961883.00153</v>
+        <v>2719453090000</v>
       </c>
       <c r="AL6" s="4">
-        <v>619111946511.62793</v>
+        <v>3567323035800</v>
       </c>
       <c r="AM6" s="4">
-        <v>564321854521.01306</v>
+        <v>4863745033400</v>
       </c>
       <c r="AN6" s="4">
-        <v>734484834573.58203</v>
+        <v>6133989133700</v>
       </c>
       <c r="AO6" s="4">
-        <v>863749314718.53784</v>
+        <v>7181362958700</v>
       </c>
       <c r="AP6" s="4">
-        <v>961601980984.62256</v>
+        <v>7971504449200</v>
       </c>
       <c r="AQ6" s="4">
-        <v>1029060747620.6549</v>
+        <v>8519550709000.001</v>
       </c>
       <c r="AR6" s="4">
-        <v>1094010482677.3937</v>
+        <v>9056437577700</v>
       </c>
       <c r="AS6" s="4">
-        <v>1211331651829.8477</v>
+        <v>10028013925300</v>
       </c>
       <c r="AT6" s="4">
-        <v>1339400897153.4365</v>
+        <v>11086312304600</v>
       </c>
       <c r="AU6" s="4">
-        <v>1470557654824.1099</v>
+        <v>12171742474800</v>
       </c>
       <c r="AV6" s="4">
-        <v>1660280543870.9529</v>
+        <v>13742203491800</v>
       </c>
       <c r="AW6" s="4">
-        <v>1955346768757.6394</v>
+        <v>16184016090700</v>
       </c>
       <c r="AX6" s="4">
-        <v>2285961149904.2568</v>
+        <v>18731890311800</v>
       </c>
       <c r="AY6" s="4">
-        <v>2752118657221.6401</v>
+        <v>21943847481700</v>
       </c>
       <c r="AZ6" s="4">
-        <v>3550327803024.6865</v>
+        <v>27009232371800</v>
       </c>
       <c r="BA6" s="4">
-        <v>4594336785752.0635</v>
+        <v>31924461277900</v>
       </c>
       <c r="BB6" s="4">
-        <v>5101691124358.4053</v>
+        <v>34851774373499.996</v>
       </c>
       <c r="BC6" s="4">
-        <v>6087191746738.5713</v>
+        <v>41211925579600</v>
       </c>
       <c r="BD6" s="4">
-        <v>7551545703518.1367</v>
+        <v>48794018052500</v>
       </c>
       <c r="BE6" s="4">
-        <v>8532185381696.4346</v>
+        <v>53857995346900</v>
       </c>
       <c r="BF6" s="4">
-        <v>9570471111847.8164</v>
+        <v>59296322954900</v>
       </c>
       <c r="BG6" s="4">
-        <v>10475624944290.115</v>
+        <v>64356310454400</v>
       </c>
       <c r="BH6" s="4">
-        <v>11061572618594.75</v>
+        <v>68885821804900.008</v>
       </c>
       <c r="BI6" s="4">
-        <v>11233313730288.52</v>
+        <v>74639505948400</v>
       </c>
       <c r="BJ6" s="4">
-        <v>12310491333980.889</v>
+        <v>83203594856000</v>
       </c>
       <c r="BK6" s="4">
-        <v>13894907857925.922</v>
+        <v>91928112906700</v>
       </c>
       <c r="BL6" s="4">
-        <v>14279968506242.775</v>
+        <v>98651520229200</v>
       </c>
       <c r="BM6" s="4">
-        <v>14687744162801.033</v>
+        <v>101356700223100</v>
       </c>
       <c r="BN6" s="4">
-        <v>17820459508852.184</v>
+        <v>114923697861100</v>
       </c>
       <c r="BO6" s="4">
-        <v>17963171479205.328</v>
-      </c>
-      <c r="BP6" s="4"/>
-      <c r="BS6" s="2"/>
+        <v>120472395261800</v>
+      </c>
+      <c r="BP6" s="4">
+        <v>126058207462620</v>
+      </c>
+      <c r="BR6" s="2"/>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2014,204 +2024,206 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4">
-        <v>147010000000</v>
+        <v>59716249310.974159</v>
       </c>
       <c r="F7" s="4">
-        <v>123230000000</v>
+        <v>50056685957.358994</v>
       </c>
       <c r="G7" s="4">
-        <v>116220000000</v>
+        <v>47209186415.355537</v>
       </c>
       <c r="H7" s="4">
-        <v>124830000000</v>
+        <v>50706614526.147232</v>
       </c>
       <c r="I7" s="4">
-        <v>146990000000</v>
+        <v>59708125203.864311</v>
       </c>
       <c r="J7" s="4">
-        <v>173400000000</v>
+        <v>70436008642.42514</v>
       </c>
       <c r="K7" s="4">
-        <v>188870000000</v>
+        <v>76720005491.896408</v>
       </c>
       <c r="L7" s="4">
-        <v>179420000000</v>
+        <v>72881364882.490875</v>
       </c>
       <c r="M7" s="4">
-        <v>174410000000</v>
+        <v>70846276051.472717</v>
       </c>
       <c r="N7" s="4">
-        <v>196220000000</v>
+        <v>79705614854.767365</v>
       </c>
       <c r="O7" s="4">
-        <v>227970000000</v>
+        <v>92602634891.658936</v>
       </c>
       <c r="P7" s="4">
-        <v>245690000000</v>
+        <v>99800593790.988647</v>
       </c>
       <c r="Q7" s="4">
-        <v>255240000000</v>
+        <v>113689308020.34328</v>
       </c>
       <c r="R7" s="4">
-        <v>275620000000</v>
+        <v>138543170458.06406</v>
       </c>
       <c r="S7" s="4">
-        <v>282770000000</v>
+        <v>144188970821.07199</v>
       </c>
       <c r="T7" s="4">
-        <v>303950000000</v>
+        <v>163429530659.63803</v>
       </c>
       <c r="U7" s="4">
-        <v>298860000000</v>
+        <v>153939265947.77521</v>
       </c>
       <c r="V7" s="4">
-        <v>325000000000</v>
+        <v>174935933078.66251</v>
       </c>
       <c r="W7" s="4">
-        <v>367870251960</v>
+        <v>149540752829.26828</v>
       </c>
       <c r="X7" s="4">
-        <v>410045367150</v>
+        <v>178280594413.04349</v>
       </c>
       <c r="Y7" s="4">
-        <v>458758107780</v>
+        <v>191149211575</v>
       </c>
       <c r="Z7" s="4">
-        <v>493583283730</v>
+        <v>195866382432.53967</v>
       </c>
       <c r="AA7" s="4">
-        <v>537335013629.99994</v>
+        <v>205089699858.77859</v>
       </c>
       <c r="AB7" s="4">
-        <v>602092410070</v>
+        <v>230686747153.25671</v>
       </c>
       <c r="AC7" s="4">
-        <v>727850230680</v>
+        <v>259946510957.14288</v>
       </c>
       <c r="AD7" s="4">
-        <v>909894802710</v>
+        <v>309488028132.65308</v>
       </c>
       <c r="AE7" s="4">
-        <v>1037615445370</v>
+        <v>300758100107.24634</v>
       </c>
       <c r="AF7" s="4">
-        <v>1217459467450</v>
+        <v>272972974764.57401</v>
       </c>
       <c r="AG7" s="4">
-        <v>1518038647670</v>
+        <v>312353631207.81891</v>
       </c>
       <c r="AH7" s="4">
-        <v>1717974173480</v>
+        <v>347768051311.74084</v>
       </c>
       <c r="AI7" s="4">
-        <v>1887286882720</v>
+        <v>360857912565.96558</v>
       </c>
       <c r="AJ7" s="4">
-        <v>2200562845800</v>
+        <v>383373318083.62366</v>
       </c>
       <c r="AK7" s="4">
-        <v>2719453090000</v>
+        <v>426915712715.85559</v>
       </c>
       <c r="AL7" s="4">
-        <v>3567323035800</v>
+        <v>444731282435.51544</v>
       </c>
       <c r="AM7" s="4">
-        <v>4863745033400</v>
+        <v>564321854521.01306</v>
       </c>
       <c r="AN7" s="4">
-        <v>6133989133700</v>
+        <v>734484834573.58203</v>
       </c>
       <c r="AO7" s="4">
-        <v>7181362958700</v>
+        <v>863749314718.53784</v>
       </c>
       <c r="AP7" s="4">
-        <v>7971504449200</v>
+        <v>961601980984.62256</v>
       </c>
       <c r="AQ7" s="4">
-        <v>8519550709000.001</v>
+        <v>1029060747620.6549</v>
       </c>
       <c r="AR7" s="4">
-        <v>9056437577700</v>
+        <v>1094003874937.3358</v>
       </c>
       <c r="AS7" s="4">
-        <v>10028013925000</v>
+        <v>1211331651866.0859</v>
       </c>
       <c r="AT7" s="4">
-        <v>11086312305000</v>
+        <v>1339400897105.1101</v>
       </c>
       <c r="AU7" s="4">
-        <v>12171742475000</v>
+        <v>1470557654799.9465</v>
       </c>
       <c r="AV7" s="4">
-        <v>13742203492000</v>
+        <v>1660280543846.7896</v>
       </c>
       <c r="AW7" s="4">
-        <v>16184016091000</v>
+        <v>1955346768721.3936</v>
       </c>
       <c r="AX7" s="4">
-        <v>18731890312000</v>
+        <v>2285961149879.8496</v>
       </c>
       <c r="AY7" s="4">
-        <v>21943847482000</v>
+        <v>2752118657184.0151</v>
       </c>
       <c r="AZ7" s="4">
-        <v>27009232372000</v>
+        <v>3550327802998.397</v>
       </c>
       <c r="BA7" s="4">
-        <v>31924461278000</v>
+        <v>4594336785737.6719</v>
       </c>
       <c r="BB7" s="4">
-        <v>34851774373999.996</v>
+        <v>5101691124285.2139</v>
       </c>
       <c r="BC7" s="4">
-        <v>41211925580000</v>
+        <v>6087191746679.4893</v>
       </c>
       <c r="BD7" s="4">
-        <v>48794018053000</v>
+        <v>7551545703440.7549</v>
       </c>
       <c r="BE7" s="4">
-        <v>53857995347000</v>
+        <v>8532185381680.5928</v>
       </c>
       <c r="BF7" s="4">
-        <v>59296322955000</v>
+        <v>9570471111831.6758</v>
       </c>
       <c r="BG7" s="4">
-        <v>64356310454000</v>
+        <v>10475624944355.225</v>
       </c>
       <c r="BH7" s="4">
-        <v>68885821805000.008</v>
+        <v>11061572618578.693</v>
       </c>
       <c r="BI7" s="4">
-        <v>74639505948000</v>
+        <v>11233313730348.719</v>
       </c>
       <c r="BJ7" s="4">
-        <v>83203594856000</v>
+        <v>12310491333980.889</v>
       </c>
       <c r="BK7" s="4">
-        <v>91928112907000</v>
+        <v>13894907857880.576</v>
       </c>
       <c r="BL7" s="4">
-        <v>98651520229000</v>
+        <v>14279968506271.727</v>
       </c>
       <c r="BM7" s="4">
-        <v>101356700223100</v>
+        <v>14687744162801.033</v>
       </c>
       <c r="BN7" s="4">
-        <v>114923697861100</v>
+        <v>17820459508852.184</v>
       </c>
       <c r="BO7" s="4">
-        <v>121020724436500</v>
-      </c>
-      <c r="BP7" s="4"/>
-      <c r="BS7" s="2"/>
+        <v>17881782683707.285</v>
+      </c>
+      <c r="BP7" s="4">
+        <v>17794783039551.957</v>
+      </c>
+      <c r="BR7" s="2"/>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2219,10 +2231,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2248,167 +2260,653 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="5">
-        <f t="shared" ref="AD8:AH8" si="0">_xlfn.FORECAST.LINEAR(AD1,$AJ$8:$AY$8,$AJ$1:$AY$1)</f>
-        <v>594470327.44558716</v>
-      </c>
-      <c r="AE8" s="5">
-        <f t="shared" si="0"/>
-        <v>603340685.55147171</v>
-      </c>
-      <c r="AF8" s="5">
-        <f t="shared" si="0"/>
-        <v>612211043.65735245</v>
-      </c>
-      <c r="AG8" s="5">
-        <f t="shared" si="0"/>
-        <v>621081401.763237</v>
-      </c>
-      <c r="AH8" s="5">
-        <f t="shared" si="0"/>
-        <v>629951759.86911774</v>
-      </c>
-      <c r="AI8" s="5">
-        <f>_xlfn.FORECAST.LINEAR(AI1,$AJ$8:$AY$8,$AJ$1:$AY$1)</f>
-        <v>638822117.97499847</v>
-      </c>
-      <c r="AJ8" s="4">
-        <v>647240828</v>
-      </c>
-      <c r="AK8" s="4">
-        <v>655427871</v>
-      </c>
-      <c r="AL8" s="4">
-        <v>663270310</v>
-      </c>
-      <c r="AM8" s="4">
-        <v>671847538</v>
-      </c>
-      <c r="AN8" s="4">
-        <v>681135001</v>
-      </c>
-      <c r="AO8" s="4">
-        <v>691090313</v>
-      </c>
-      <c r="AP8" s="4">
-        <v>702212322</v>
-      </c>
-      <c r="AQ8" s="4">
-        <v>712827235</v>
-      </c>
-      <c r="AR8" s="4">
-        <v>722366758</v>
-      </c>
-      <c r="AS8" s="4">
-        <v>731993935</v>
-      </c>
-      <c r="AT8" s="4">
-        <v>739359562</v>
-      </c>
-      <c r="AU8" s="4">
-        <v>747567965</v>
-      </c>
-      <c r="AV8" s="4">
-        <v>755273046</v>
-      </c>
-      <c r="AW8" s="4">
-        <v>762251057</v>
-      </c>
-      <c r="AX8" s="4">
-        <v>769371812</v>
-      </c>
-      <c r="AY8" s="4">
-        <v>774287037</v>
-      </c>
-      <c r="AZ8" s="4">
-        <v>776045127</v>
-      </c>
-      <c r="BA8" s="4">
-        <v>776378230</v>
-      </c>
-      <c r="BB8" s="4">
-        <v>775599063</v>
-      </c>
-      <c r="BC8" s="4">
-        <v>774058132</v>
-      </c>
-      <c r="BD8" s="4">
-        <v>778323480</v>
-      </c>
-      <c r="BE8" s="4">
-        <v>778937997</v>
-      </c>
-      <c r="BF8" s="4">
-        <v>779042510</v>
-      </c>
-      <c r="BG8" s="4">
-        <v>780062420</v>
-      </c>
-      <c r="BH8" s="4">
-        <v>780709584</v>
-      </c>
-      <c r="BI8" s="4">
-        <v>780524312</v>
-      </c>
-      <c r="BJ8" s="4">
-        <v>778674707</v>
-      </c>
-      <c r="BK8" s="4">
-        <v>776278514</v>
-      </c>
-      <c r="BL8" s="4">
-        <v>775321104</v>
-      </c>
-      <c r="BM8" s="4">
-        <v>763684716</v>
-      </c>
-      <c r="BN8" s="4">
-        <v>780370660</v>
-      </c>
-      <c r="BO8" s="4">
-        <v>781808304</v>
-      </c>
-      <c r="BP8" s="4">
-        <v>779890786</v>
-      </c>
-      <c r="BQ8" t="s">
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="6"/>
+      <c r="AV8" s="6"/>
+      <c r="AW8" s="6"/>
+      <c r="AX8" s="6"/>
+      <c r="AY8" s="6"/>
+      <c r="AZ8" s="6"/>
+      <c r="BA8" s="6"/>
+      <c r="BB8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="6"/>
+      <c r="BF8" s="6"/>
+      <c r="BG8" s="6"/>
+      <c r="BH8" s="6">
+        <v>4656294690492.4277</v>
+      </c>
+      <c r="BI8" s="4"/>
+      <c r="BJ8" s="4"/>
+      <c r="BK8" s="4"/>
+      <c r="BL8" s="4"/>
+      <c r="BM8" s="4"/>
+      <c r="BN8" s="4"/>
+      <c r="BO8" s="4"/>
+      <c r="BP8" s="4"/>
+      <c r="BR8" s="2"/>
+    </row>
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP9" s="4"/>
+      <c r="BR9" s="2"/>
+    </row>
+    <row r="10" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>47993387760</v>
+      </c>
+      <c r="F10" s="4">
+        <v>23402925930</v>
+      </c>
+      <c r="G10" s="4">
+        <v>17989913990</v>
+      </c>
+      <c r="H10" s="4">
+        <v>22165333630</v>
+      </c>
+      <c r="I10" s="4">
+        <v>29788307220</v>
+      </c>
+      <c r="J10" s="4">
+        <v>35793882630</v>
+      </c>
+      <c r="K10" s="4">
+        <v>41219319890</v>
+      </c>
+      <c r="L10" s="4">
+        <v>32614267800</v>
+      </c>
+      <c r="M10" s="4">
+        <v>30289799040</v>
+      </c>
+      <c r="N10" s="4">
+        <v>41172135460</v>
+      </c>
+      <c r="O10" s="4">
+        <v>55032546060</v>
+      </c>
+      <c r="P10" s="4">
+        <v>61044779800</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>62858199860</v>
+      </c>
+      <c r="R10" s="4">
+        <v>66933391619.999992</v>
+      </c>
+      <c r="S10" s="4">
+        <v>75097156030</v>
+      </c>
+      <c r="T10" s="4">
+        <v>88291066570</v>
+      </c>
+      <c r="U10" s="4">
+        <v>86780576550</v>
+      </c>
+      <c r="V10" s="4">
+        <v>91406619870</v>
+      </c>
+      <c r="W10" s="4">
+        <v>107933244300</v>
+      </c>
+      <c r="X10" s="4">
+        <v>116253769680</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>131024128950</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>134539520040</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>151740287720</v>
+      </c>
+      <c r="AB10" s="4">
+        <v>169653197290</v>
+      </c>
+      <c r="AC10" s="4">
+        <v>213413308470</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>276892278350</v>
+      </c>
+      <c r="AE10" s="4">
+        <v>321241196560</v>
+      </c>
+      <c r="AF10" s="4">
+        <v>372036584180</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>471393839400</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>439905629200</v>
+      </c>
+      <c r="AI10" s="4">
+        <v>452736600850</v>
+      </c>
+      <c r="AJ10" s="4">
+        <v>565628247500</v>
+      </c>
+      <c r="AK10" s="4">
+        <v>825281121800</v>
+      </c>
+      <c r="AL10" s="4">
+        <v>1323199771900</v>
+      </c>
+      <c r="AM10" s="4">
+        <v>1675103770600</v>
+      </c>
+      <c r="AN10" s="4">
+        <v>1983791512300</v>
+      </c>
+      <c r="AO10" s="4">
+        <v>2272327207700</v>
+      </c>
+      <c r="AP10" s="4">
+        <v>2471413193200</v>
+      </c>
+      <c r="AQ10" s="4">
+        <v>2801449320000</v>
+      </c>
+      <c r="AR10" s="4">
+        <v>2946704495500</v>
+      </c>
+      <c r="AS10" s="4">
+        <v>3266867972500</v>
+      </c>
+      <c r="AT10" s="4">
+        <v>3708762410400</v>
+      </c>
+      <c r="AU10" s="4">
+        <v>4267214031700</v>
+      </c>
+      <c r="AV10" s="4">
+        <v>5257448969100</v>
+      </c>
+      <c r="AW10" s="4">
+        <v>6397487138200</v>
+      </c>
+      <c r="AX10" s="4">
+        <v>7385200526700</v>
+      </c>
+      <c r="AY10" s="4">
+        <v>8497862046100</v>
+      </c>
+      <c r="AZ10" s="4">
+        <v>10234464824700</v>
+      </c>
+      <c r="BA10" s="4">
+        <v>12470070672900</v>
+      </c>
+      <c r="BB10" s="4">
+        <v>15269109881000</v>
+      </c>
+      <c r="BC10" s="4">
+        <v>18104112388800</v>
+      </c>
+      <c r="BD10" s="4">
+        <v>21401720630600</v>
+      </c>
+      <c r="BE10" s="4">
+        <v>23832072453600</v>
+      </c>
+      <c r="BF10" s="4">
+        <v>26397990996200</v>
+      </c>
+      <c r="BG10" s="4">
+        <v>28224163815700</v>
+      </c>
+      <c r="BH10" s="4">
+        <v>28997023965800</v>
+      </c>
+      <c r="BI10" s="4">
+        <v>31014479887600</v>
+      </c>
+      <c r="BJ10" s="4">
+        <v>34830011017200</v>
+      </c>
+      <c r="BK10" s="4">
+        <v>39384790035500</v>
+      </c>
+      <c r="BL10" s="4">
+        <v>42245130463600</v>
+      </c>
+      <c r="BM10" s="4">
+        <v>43062487270000</v>
+      </c>
+      <c r="BN10" s="4">
+        <v>48211932377800</v>
+      </c>
+      <c r="BO10" s="4">
+        <v>50483464386770</v>
+      </c>
+      <c r="BP10" s="4">
+        <v>52111231473800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4">
+        <v>19495171136.347294</v>
+      </c>
+      <c r="F11" s="4">
+        <v>9506393846.9637566</v>
+      </c>
+      <c r="G11" s="4">
+        <v>7307599407.5901089</v>
+      </c>
+      <c r="H11" s="4">
+        <v>9003677226.7872925</v>
+      </c>
+      <c r="I11" s="4">
+        <v>12100169923.824308</v>
+      </c>
+      <c r="J11" s="4">
+        <v>14539666818.181263</v>
+      </c>
+      <c r="K11" s="4">
+        <v>16743508489.082621</v>
+      </c>
+      <c r="L11" s="4">
+        <v>13248090245.831419</v>
+      </c>
+      <c r="M11" s="4">
+        <v>12303878586.844065</v>
+      </c>
+      <c r="N11" s="4">
+        <v>16724341920.920753</v>
+      </c>
+      <c r="O11" s="4">
+        <v>22354514935.967819</v>
+      </c>
+      <c r="P11" s="4">
+        <v>24796716479.62941</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>27998375041.090107</v>
+      </c>
+      <c r="R11" s="4">
+        <v>33644743794.158684</v>
+      </c>
+      <c r="S11" s="4">
+        <v>38293247655.533333</v>
+      </c>
+      <c r="T11" s="4">
+        <v>47472832936.252533</v>
+      </c>
+      <c r="U11" s="4">
+        <v>44699652856.292961</v>
+      </c>
+      <c r="V11" s="4">
+        <v>49200930266.230957</v>
+      </c>
+      <c r="W11" s="4">
+        <v>43875302560.975609</v>
+      </c>
+      <c r="X11" s="4">
+        <v>50545117252.17392</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>54593387062.5</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>53388698428.571426</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>57916140351.145035</v>
+      </c>
+      <c r="AB11" s="4">
+        <v>65001225015.325676</v>
+      </c>
+      <c r="AC11" s="4">
+        <v>76219038739.285721</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>94181047057.823135</v>
+      </c>
+      <c r="AE11" s="4">
+        <v>93113390307.246368</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>83416274479.820633</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>96994617160.49382</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>89049722510.121445</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>86565315650.095596</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>98541506533.101044</v>
+      </c>
+      <c r="AK11" s="4">
+        <v>129557475949.76453</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>164960763454.80157</v>
+      </c>
+      <c r="AM11" s="4">
+        <v>194355925289.80154</v>
+      </c>
+      <c r="AN11" s="4">
+        <v>237539511235.03952</v>
+      </c>
+      <c r="AO11" s="4">
+        <v>273307599094.31781</v>
+      </c>
+      <c r="AP11" s="4">
+        <v>298126387253.18066</v>
+      </c>
+      <c r="AQ11" s="4">
+        <v>338381873660.91241</v>
+      </c>
+      <c r="AR11" s="4">
+        <v>355957417992.93329</v>
+      </c>
+      <c r="AS11" s="4">
+        <v>394620570636.91699</v>
+      </c>
+      <c r="AT11" s="4">
+        <v>448076832327.5827</v>
+      </c>
+      <c r="AU11" s="4">
+        <v>515553485622.79596</v>
+      </c>
+      <c r="AV11" s="4">
+        <v>635184906035.81934</v>
+      </c>
+      <c r="AW11" s="4">
+        <v>772942002375.07214</v>
+      </c>
+      <c r="AX11" s="4">
+        <v>901258826904.06042</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>1065771383197.5618</v>
+      </c>
+      <c r="AZ11" s="4">
+        <v>1345306838630.4521</v>
+      </c>
+      <c r="BA11" s="4">
+        <v>1794602073768.2329</v>
+      </c>
+      <c r="BB11" s="4">
+        <v>2235131030082.1968</v>
+      </c>
+      <c r="BC11" s="4">
+        <v>2674061014237.396</v>
+      </c>
+      <c r="BD11" s="4">
+        <v>3312210757071.814</v>
+      </c>
+      <c r="BE11" s="4">
+        <v>3775477696376.2847</v>
+      </c>
+      <c r="BF11" s="4">
+        <v>4260655596328.9727</v>
+      </c>
+      <c r="BG11" s="4">
+        <v>4594199891412.5225</v>
+      </c>
+      <c r="BH11" s="4">
+        <v>4656294690492.4277</v>
+      </c>
+      <c r="BI11" s="4">
+        <v>4667707514059.043</v>
+      </c>
+      <c r="BJ11" s="4">
+        <v>5153317588402.0059</v>
+      </c>
+      <c r="BK11" s="4">
+        <v>5952999699892.2451</v>
+      </c>
+      <c r="BL11" s="4">
+        <v>6115051558880.9834</v>
+      </c>
+      <c r="BM11" s="4">
+        <v>6240246521872.1338</v>
+      </c>
+      <c r="BN11" s="4">
+        <v>7475906229718.6768</v>
+      </c>
+      <c r="BO11" s="4">
+        <v>7493287879959.1758</v>
+      </c>
+      <c r="BP11" s="4">
+        <v>7356189467275.3994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W12" s="5">
+        <v>557681546.19999886</v>
+      </c>
+      <c r="X12" s="5">
+        <v>564440815.15757561</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>571200084.11515045</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>577959353.0727272</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>584718622.03030205</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>591477890.9878788</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>598237159.94545364</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>604996428.9030304</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>611755697.86060524</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>618514966.81818199</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>625274235.77575684</v>
+      </c>
+      <c r="AH12" s="5">
+        <v>632033504.73333359</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>639912098</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>646245556</v>
+      </c>
+      <c r="AK12" s="4">
+        <v>652547071</v>
+      </c>
+      <c r="AL12" s="4">
+        <v>658329022</v>
+      </c>
+      <c r="AM12" s="4">
+        <v>664565882</v>
+      </c>
+      <c r="AN12" s="4">
+        <v>671238114</v>
+      </c>
+      <c r="AO12" s="4">
+        <v>678359927</v>
+      </c>
+      <c r="AP12" s="4">
+        <v>686473251</v>
+      </c>
+      <c r="AQ12" s="4">
+        <v>694001983</v>
+      </c>
+      <c r="AR12" s="4">
+        <v>700421936</v>
+      </c>
+      <c r="AS12" s="4">
+        <v>706837950</v>
+      </c>
+      <c r="AT12" s="4">
+        <v>715928584</v>
+      </c>
+      <c r="AU12" s="4">
+        <v>725938760</v>
+      </c>
+      <c r="AV12" s="4">
+        <v>735682023</v>
+      </c>
+      <c r="AW12" s="4">
+        <v>744936890</v>
+      </c>
+      <c r="AX12" s="4">
+        <v>754465388</v>
+      </c>
+      <c r="AY12" s="4">
+        <v>761948735</v>
+      </c>
+      <c r="AZ12" s="4">
+        <v>766486940</v>
+      </c>
+      <c r="BA12" s="4">
+        <v>769779554</v>
+      </c>
+      <c r="BB12" s="4">
+        <v>772141043</v>
+      </c>
+      <c r="BC12" s="4">
+        <v>773873234</v>
+      </c>
+      <c r="BD12" s="4">
+        <v>778275581</v>
+      </c>
+      <c r="BE12" s="4">
+        <v>779022561</v>
+      </c>
+      <c r="BF12" s="4">
+        <v>779251311</v>
+      </c>
+      <c r="BG12" s="4">
+        <v>780370287</v>
+      </c>
+      <c r="BH12" s="4">
+        <v>781077009</v>
+      </c>
+      <c r="BI12" s="4">
+        <v>780932880</v>
+      </c>
+      <c r="BJ12" s="4">
+        <v>779166682</v>
+      </c>
+      <c r="BK12" s="4">
+        <v>776868988</v>
+      </c>
+      <c r="BL12" s="4">
+        <v>775928449</v>
+      </c>
+      <c r="BM12" s="4">
+        <v>763830073</v>
+      </c>
+      <c r="BN12" s="4">
+        <v>781187865</v>
+      </c>
+      <c r="BO12" s="4">
+        <v>770113477</v>
+      </c>
+      <c r="BP12" s="4">
+        <v>774607590</v>
+      </c>
+      <c r="BQ12" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="BS8" s="2"/>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS9" s="2"/>
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BR13" s="2"/>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS10" s="2"/>
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BR14" s="2"/>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS11" s="2"/>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BR15" s="2"/>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS12" s="2"/>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BR16" s="2"/>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS13" s="2"/>
+    <row r="17" spans="70:70" x14ac:dyDescent="0.25">
+      <c r="BR17" s="2"/>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS14" s="2"/>
+    <row r="18" spans="70:70" x14ac:dyDescent="0.25">
+      <c r="BR18" s="2"/>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS15" s="2"/>
-    </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="BS16" s="2"/>
-    </row>
-    <row r="17" spans="71:71" x14ac:dyDescent="0.25">
-      <c r="BS17" s="2"/>
-    </row>
-    <row r="18" spans="71:71" x14ac:dyDescent="0.25">
-      <c r="BS18" s="2"/>
-    </row>
-    <row r="19" spans="71:71" x14ac:dyDescent="0.25">
-      <c r="BS19" s="2"/>
+    <row r="19" spans="70:70" x14ac:dyDescent="0.25">
+      <c r="BR19" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:BQ8">

</xml_diff>